<commit_message>
fixing a couple of problems and missing vocab
</commit_message>
<xml_diff>
--- a/keim-nane-vocabulary.xlsx
+++ b/keim-nane-vocabulary.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D269"/>
+  <dimension ref="A1:D270"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6283,6 +6283,28 @@
         </is>
       </c>
     </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>jerrey-shiaghtin</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>weekend</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Nouns</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>